<commit_message>
Add parameters names description to model parameters
</commit_message>
<xml_diff>
--- a/Data/Model parameters.xlsx
+++ b/Data/Model parameters.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinekrijkamp/Documents/GitHub/Utilitarian-distribution-of-OR-capacity-during-COVID-19/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F641F66-025B-AF4E-9753-8EAC3232A25F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC606FF-D6DB-2348-8160-7057A36F744A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="0" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="940" yWindow="0" windowWidth="23260" windowHeight="12580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Complete" sheetId="1" r:id="rId1"/>
+    <sheet name="Parameter names" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2646" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2664" uniqueCount="250">
   <si>
     <t>Tx_eff</t>
   </si>
@@ -745,13 +746,43 @@
   </si>
   <si>
     <t>Patients with mild laryngeal cancer</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definition </t>
+  </si>
+  <si>
+    <t>Average of of the patient population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The quality of life of the patients before the surgery </t>
+  </si>
+  <si>
+    <t>The quality of life of the patients after the surgery</t>
+  </si>
+  <si>
+    <t>The expected survival of the patients before the surgery</t>
+  </si>
+  <si>
+    <t>The expected survival of the patients after the surgery</t>
+  </si>
+  <si>
+    <t>The time until no effect on the survival is expected anymore by the surgery</t>
+  </si>
+  <si>
+    <t>The treatment effect of the surgery</t>
+  </si>
+  <si>
+    <t>The time until no effect on the quality of life is expeceted by surgery</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -791,6 +822,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -811,11 +850,20 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -824,7 +872,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -854,6 +902,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent6" xfId="1" builtinId="49"/>
@@ -1170,11 +1220,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1448"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B177" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="81" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A192" sqref="A192"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D2:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22286,4 +22336,94 @@
     <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C74CB41-3A12-2141-8820-AE0993798E54}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>249</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>